<commit_message>
Refactor5: setting print kaf005 v3
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF005_残業申請\UK2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UkSource\UniversalK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -72,7 +72,7 @@
     <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
     <definedName name="関連表" hidden="1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -455,26 +455,35 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -493,18 +502,9 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準 10" xfId="2"/>
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="4"/>
@@ -550,7 +550,7 @@
         <xdr:cNvPr id="2" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -569,7 +569,7 @@
           <xdr:cNvPr id="3" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -623,7 +623,7 @@
           <xdr:cNvPr id="4" name="直線コネクタ 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -663,7 +663,7 @@
           <xdr:cNvPr id="5" name="直線コネクタ 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -703,7 +703,7 @@
           <xdr:cNvPr id="6" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -759,7 +759,7 @@
           <xdr:cNvPr id="7" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -822,7 +822,7 @@
           <xdr:cNvPr id="8" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -901,7 +901,7 @@
         <xdr:cNvPr id="9" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -920,7 +920,7 @@
           <xdr:cNvPr id="10" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -974,7 +974,7 @@
           <xdr:cNvPr id="11" name="直線コネクタ 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1014,7 +1014,7 @@
           <xdr:cNvPr id="12" name="直線コネクタ 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1054,7 +1054,7 @@
           <xdr:cNvPr id="13" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1110,7 +1110,7 @@
           <xdr:cNvPr id="14" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1166,7 +1166,7 @@
           <xdr:cNvPr id="15" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1238,7 +1238,7 @@
         <xdr:cNvPr id="16" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1257,7 +1257,7 @@
           <xdr:cNvPr id="17" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1311,7 +1311,7 @@
           <xdr:cNvPr id="18" name="直線コネクタ 17">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1351,7 +1351,7 @@
           <xdr:cNvPr id="19" name="直線コネクタ 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1391,7 +1391,7 @@
           <xdr:cNvPr id="20" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1447,7 +1447,7 @@
           <xdr:cNvPr id="21" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1510,7 +1510,7 @@
           <xdr:cNvPr id="22" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1582,7 +1582,7 @@
         <xdr:cNvPr id="23" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1601,7 +1601,7 @@
           <xdr:cNvPr id="24" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1655,7 +1655,7 @@
           <xdr:cNvPr id="25" name="直線コネクタ 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1695,7 +1695,7 @@
           <xdr:cNvPr id="26" name="直線コネクタ 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1735,7 +1735,7 @@
           <xdr:cNvPr id="27" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1791,7 +1791,7 @@
           <xdr:cNvPr id="28" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1847,7 +1847,7 @@
           <xdr:cNvPr id="29" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1919,7 +1919,7 @@
         <xdr:cNvPr id="30" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1938,7 +1938,7 @@
           <xdr:cNvPr id="31" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1992,7 +1992,7 @@
           <xdr:cNvPr id="32" name="直線コネクタ 31">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2032,7 +2032,7 @@
           <xdr:cNvPr id="33" name="直線コネクタ 32">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2072,7 +2072,7 @@
           <xdr:cNvPr id="34" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2128,7 +2128,7 @@
           <xdr:cNvPr id="35" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2191,7 +2191,7 @@
           <xdr:cNvPr id="36" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2637,7 +2637,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
@@ -2673,10 +2673,10 @@
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="34"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2687,10 +2687,10 @@
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="34"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="51"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2714,8 +2714,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -2728,8 +2728,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="53"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -2798,8 +2798,8 @@
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="50"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="53"/>
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
@@ -2812,8 +2812,8 @@
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="50"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
       <c r="D13" s="13"/>
       <c r="E13" s="14"/>
       <c r="F13" s="13"/>
@@ -2826,8 +2826,8 @@
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="13"/>
       <c r="E14" s="14"/>
       <c r="F14" s="13"/>
@@ -2840,8 +2840,8 @@
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="13"/>
       <c r="E15" s="14"/>
       <c r="F15" s="13"/>
@@ -2854,8 +2854,8 @@
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="13"/>
       <c r="E16" s="14"/>
       <c r="F16" s="13"/>
@@ -2868,8 +2868,8 @@
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="41"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="13"/>
       <c r="E17" s="14"/>
       <c r="F17" s="13"/>
@@ -2882,8 +2882,8 @@
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
       <c r="D18" s="13"/>
       <c r="E18" s="14"/>
       <c r="F18" s="10"/>
@@ -2896,8 +2896,8 @@
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="53"/>
       <c r="D19" s="13"/>
       <c r="E19" s="14"/>
       <c r="F19" s="13"/>
@@ -2910,8 +2910,8 @@
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="13"/>
       <c r="E20" s="14"/>
       <c r="F20" s="13"/>
@@ -2924,8 +2924,8 @@
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="13"/>
       <c r="E21" s="14"/>
       <c r="F21" s="13"/>
@@ -2938,8 +2938,8 @@
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="13"/>
       <c r="E22" s="14"/>
       <c r="F22" s="13"/>
@@ -2952,8 +2952,8 @@
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="13"/>
       <c r="E23" s="14"/>
       <c r="F23" s="13"/>
@@ -2966,8 +2966,8 @@
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="13"/>
       <c r="E24" s="14"/>
       <c r="F24" s="10"/>
@@ -2980,198 +2980,198 @@
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="13"/>
       <c r="E25" s="14"/>
       <c r="F25" s="13"/>
       <c r="G25" s="16"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="37"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="39"/>
       <c r="J25" s="15"/>
       <c r="K25" s="16"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="3.75" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="21"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="47"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="90" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="46"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="26"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="3.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="26"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="21"/>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" ht="3.75" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="21"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="47"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="46"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="26"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="3.75" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="26"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="29"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="3.75" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="29"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="55"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="32"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" ht="3.75" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="32"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="29"/>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" ht="3.75" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="29"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="44"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" ht="74.25" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="54"/>
-      <c r="K37" s="55"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="32"/>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" ht="3.75" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="32"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
       <c r="L38" s="1"/>
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1">
@@ -3260,16 +3260,16 @@
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1">
       <c r="A45" s="1"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
       <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1">
@@ -3344,18 +3344,7 @@
       <c r="J51" s="33"/>
       <c r="K51" s="33"/>
     </row>
-    <row r="52" spans="2:11" ht="15" customHeight="1">
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="33"/>
-      <c r="J52" s="33"/>
-      <c r="K52" s="33"/>
-    </row>
+    <row r="52" spans="2:11" ht="15" customHeight="1"/>
     <row r="53" spans="2:11" ht="15" customHeight="1"/>
     <row r="54" spans="2:11" ht="15" customHeight="1"/>
     <row r="55" spans="2:11" ht="15" customHeight="1"/>
@@ -3366,16 +3355,14 @@
     <row r="60" spans="2:11" ht="15" customHeight="1"/>
     <row r="61" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:K37"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:K31"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:K34"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:K28"/>
-    <mergeCell ref="B26:C26"/>
+  <mergeCells count="26">
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:K27"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:F4"/>
@@ -3389,11 +3376,12 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:K33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Refactor5: Update Print KAF005B
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UkSource\UniversalK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF005_残業申請\UK2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27405" windowHeight="14130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23145" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="残業申請" sheetId="29" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <definedName name="kkkk" hidden="1">#REF!</definedName>
     <definedName name="ｌ" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ｌ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">残業申請!$A$1:$L$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">残業申請!$A$1:$L$38</definedName>
     <definedName name="sss" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="sss" hidden="1">#REF!</definedName>
     <definedName name="Ver002001006特休残管理対応" localSheetId="0" hidden="1">#REF!</definedName>
@@ -72,7 +72,7 @@
     <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
     <definedName name="関連表" hidden="1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -333,7 +333,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -445,30 +445,27 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="20" fontId="5" fillId="2" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="5" fillId="2" borderId="12" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="20" fontId="5" fillId="2" borderId="11" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -478,12 +475,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -504,7 +495,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 10" xfId="2"/>
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="4"/>
@@ -550,7 +541,7 @@
         <xdr:cNvPr id="2" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -569,7 +560,7 @@
           <xdr:cNvPr id="3" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -623,7 +614,7 @@
           <xdr:cNvPr id="4" name="直線コネクタ 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -663,7 +654,7 @@
           <xdr:cNvPr id="5" name="直線コネクタ 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -703,7 +694,7 @@
           <xdr:cNvPr id="6" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -759,7 +750,7 @@
           <xdr:cNvPr id="7" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -822,7 +813,7 @@
           <xdr:cNvPr id="8" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -901,7 +892,7 @@
         <xdr:cNvPr id="9" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -920,7 +911,7 @@
           <xdr:cNvPr id="10" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -974,7 +965,7 @@
           <xdr:cNvPr id="11" name="直線コネクタ 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1014,7 +1005,7 @@
           <xdr:cNvPr id="12" name="直線コネクタ 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1054,7 +1045,7 @@
           <xdr:cNvPr id="13" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1110,7 +1101,7 @@
           <xdr:cNvPr id="14" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1166,7 +1157,7 @@
           <xdr:cNvPr id="15" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1238,7 +1229,7 @@
         <xdr:cNvPr id="16" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1257,7 +1248,7 @@
           <xdr:cNvPr id="17" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1311,7 +1302,7 @@
           <xdr:cNvPr id="18" name="直線コネクタ 17">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1351,7 +1342,7 @@
           <xdr:cNvPr id="19" name="直線コネクタ 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1391,7 +1382,7 @@
           <xdr:cNvPr id="20" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1447,7 +1438,7 @@
           <xdr:cNvPr id="21" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1510,7 +1501,7 @@
           <xdr:cNvPr id="22" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1582,7 +1573,7 @@
         <xdr:cNvPr id="23" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1601,7 +1592,7 @@
           <xdr:cNvPr id="24" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1655,7 +1646,7 @@
           <xdr:cNvPr id="25" name="直線コネクタ 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1695,7 +1686,7 @@
           <xdr:cNvPr id="26" name="直線コネクタ 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1735,7 +1726,7 @@
           <xdr:cNvPr id="27" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1791,7 +1782,7 @@
           <xdr:cNvPr id="28" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1847,7 +1838,7 @@
           <xdr:cNvPr id="29" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1919,7 +1910,7 @@
         <xdr:cNvPr id="30" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1938,7 +1929,7 @@
           <xdr:cNvPr id="31" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1992,7 +1983,7 @@
           <xdr:cNvPr id="32" name="直線コネクタ 31">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2032,7 +2023,7 @@
           <xdr:cNvPr id="33" name="直線コネクタ 32">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2072,7 +2063,7 @@
           <xdr:cNvPr id="34" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2128,7 +2119,7 @@
           <xdr:cNvPr id="35" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2191,7 +2182,7 @@
           <xdr:cNvPr id="36" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2634,10 +2625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
@@ -2673,10 +2664,10 @@
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="34"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="48"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2687,10 +2678,10 @@
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="34"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="51"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2714,8 +2705,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -2728,8 +2719,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -2798,8 +2789,8 @@
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="53"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
@@ -2812,187 +2803,187 @@
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="16"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="39"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="16"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="16"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="39"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="16"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="39"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="16"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="39"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="16"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="16"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="39"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="16"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="39"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="16"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="39"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="16"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="39"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="16"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="39"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="16"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="39"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="16"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="39"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="39"/>
+      <c r="I25" s="37"/>
       <c r="J25" s="15"/>
       <c r="K25" s="16"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="30" customHeight="1">
+    <row r="26" spans="1:12" ht="3.75" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
@@ -3006,21 +2997,21 @@
       <c r="K26" s="21"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" ht="3.75" customHeight="1">
+    <row r="27" spans="1:12" ht="90" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="47"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="46"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="90" customHeight="1">
+    <row r="28" spans="1:12" ht="3.75" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="22"/>
       <c r="C28" s="23"/>
@@ -3048,21 +3039,21 @@
       <c r="K29" s="21"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="3.75" customHeight="1">
+    <row r="30" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="47"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="46"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" ht="39.950000000000003" customHeight="1">
+    <row r="31" spans="1:12" ht="3.75" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="22"/>
       <c r="C31" s="23"/>
@@ -3090,21 +3081,21 @@
       <c r="K32" s="29"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" ht="3.75" customHeight="1">
+    <row r="33" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="44"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="46"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="39.950000000000003" customHeight="1">
+    <row r="34" spans="1:12" ht="3.75" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="22"/>
       <c r="C34" s="23"/>
@@ -3132,21 +3123,21 @@
       <c r="K35" s="29"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" ht="3.75" customHeight="1">
+    <row r="36" spans="1:12" ht="74.25" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="44"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="46"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" ht="74.25" customHeight="1">
+    <row r="37" spans="1:12" ht="3.75" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="22"/>
       <c r="C37" s="23"/>
@@ -3160,7 +3151,7 @@
       <c r="K37" s="32"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" ht="3.75" customHeight="1">
+    <row r="38" spans="1:12" ht="15" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -3259,7 +3250,6 @@
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1">
-      <c r="A45" s="1"/>
       <c r="B45" s="33"/>
       <c r="C45" s="33"/>
       <c r="D45" s="33"/>
@@ -3270,7 +3260,6 @@
       <c r="I45" s="33"/>
       <c r="J45" s="33"/>
       <c r="K45" s="33"/>
-      <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1">
       <c r="B46" s="33"/>
@@ -3353,17 +3342,18 @@
     <row r="58" spans="2:11" ht="15" customHeight="1"/>
     <row r="59" spans="2:11" ht="15" customHeight="1"/>
     <row r="60" spans="2:11" ht="15" customHeight="1"/>
-    <row r="61" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
+  <mergeCells count="76">
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:K33"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:K27"/>
     <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="B6:C6"/>
@@ -3376,12 +3366,60 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:K36"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:K30"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:K33"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>
@@ -3392,7 +3430,7 @@
 </oddHeader>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="29" max="11" man="1"/>
+    <brk id="28" max="11" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor5: Change template print KAF005 v1
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF005_残業申請\UK2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UkSource\UniversalK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -72,7 +72,7 @@
     <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
     <definedName name="関連表" hidden="1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -81,8 +81,16 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="1">
+  <si>
+    <t>g</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -333,7 +341,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -376,9 +384,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="20" fontId="5" fillId="2" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -448,54 +453,63 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="11" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準 10" xfId="2"/>
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="4"/>
@@ -541,7 +555,7 @@
         <xdr:cNvPr id="2" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -560,7 +574,7 @@
           <xdr:cNvPr id="3" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -614,7 +628,7 @@
           <xdr:cNvPr id="4" name="直線コネクタ 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -654,7 +668,7 @@
           <xdr:cNvPr id="5" name="直線コネクタ 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -694,7 +708,7 @@
           <xdr:cNvPr id="6" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -750,7 +764,7 @@
           <xdr:cNvPr id="7" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -813,7 +827,7 @@
           <xdr:cNvPr id="8" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -892,7 +906,7 @@
         <xdr:cNvPr id="9" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -911,7 +925,7 @@
           <xdr:cNvPr id="10" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -965,7 +979,7 @@
           <xdr:cNvPr id="11" name="直線コネクタ 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1005,7 +1019,7 @@
           <xdr:cNvPr id="12" name="直線コネクタ 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1045,7 +1059,7 @@
           <xdr:cNvPr id="13" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1101,7 +1115,7 @@
           <xdr:cNvPr id="14" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1157,7 +1171,7 @@
           <xdr:cNvPr id="15" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1229,7 +1243,7 @@
         <xdr:cNvPr id="16" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1248,7 +1262,7 @@
           <xdr:cNvPr id="17" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1302,7 +1316,7 @@
           <xdr:cNvPr id="18" name="直線コネクタ 17">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1342,7 +1356,7 @@
           <xdr:cNvPr id="19" name="直線コネクタ 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1382,7 +1396,7 @@
           <xdr:cNvPr id="20" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1438,7 +1452,7 @@
           <xdr:cNvPr id="21" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1501,7 +1515,7 @@
           <xdr:cNvPr id="22" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1573,7 +1587,7 @@
         <xdr:cNvPr id="23" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1592,7 +1606,7 @@
           <xdr:cNvPr id="24" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1646,7 +1660,7 @@
           <xdr:cNvPr id="25" name="直線コネクタ 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1686,7 +1700,7 @@
           <xdr:cNvPr id="26" name="直線コネクタ 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1726,7 +1740,7 @@
           <xdr:cNvPr id="27" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1782,7 +1796,7 @@
           <xdr:cNvPr id="28" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1838,7 +1852,7 @@
           <xdr:cNvPr id="29" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1910,7 +1924,7 @@
         <xdr:cNvPr id="30" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1929,7 +1943,7 @@
           <xdr:cNvPr id="31" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1983,7 +1997,7 @@
           <xdr:cNvPr id="32" name="直線コネクタ 31">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2023,7 +2037,7 @@
           <xdr:cNvPr id="33" name="直線コネクタ 32">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2063,7 +2077,7 @@
           <xdr:cNvPr id="34" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2119,7 +2133,7 @@
           <xdr:cNvPr id="35" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2182,7 +2196,7 @@
           <xdr:cNvPr id="36" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2627,8 +2641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
@@ -2663,11 +2677,11 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2677,11 +2691,11 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2705,8 +2719,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -2719,8 +2733,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -2733,422 +2747,436 @@
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="16"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="16"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="54" t="s">
+        <v>0</v>
+      </c>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="39"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="51"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="51"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="39"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="51"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="51"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="39"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="51"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="51"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="39"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="51"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="39"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="51"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="39"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="51"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="39"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="51"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="39"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="51"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="39"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="51"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="39"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="51"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="16"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="3.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="90" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="46"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="41"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="3.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="26"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="25"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="3.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="21"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="20"/>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="46"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="41"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="3.75" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="26"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="25"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="3.75" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="29"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="28"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="46"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="41"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="3.75" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="32"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="31"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" ht="3.75" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="29"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="28"/>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" ht="74.25" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="46"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="41"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" ht="3.75" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="32"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="31"/>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1">
@@ -3250,88 +3278,88 @@
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1">
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="33"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1">
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="33"/>
-      <c r="J46" s="33"/>
-      <c r="K46" s="33"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1">
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="33"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="32"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1">
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
     </row>
     <row r="49" spans="2:11" ht="15" customHeight="1">
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="33"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="33"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
     </row>
     <row r="50" spans="2:11" ht="15" customHeight="1">
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="33"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32"/>
     </row>
     <row r="51" spans="2:11" ht="15" customHeight="1">
-      <c r="B51" s="33"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="33"/>
-      <c r="J51" s="33"/>
-      <c r="K51" s="33"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32"/>
     </row>
     <row r="52" spans="2:11" ht="15" customHeight="1"/>
     <row r="53" spans="2:11" ht="15" customHeight="1"/>
@@ -3343,13 +3371,62 @@
     <row r="59" spans="2:11" ht="15" customHeight="1"/>
     <row r="60" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:K36"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:K30"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:K33"/>
+  <mergeCells count="77">
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:K27"/>
     <mergeCell ref="B25:C25"/>
@@ -3366,60 +3443,12 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:K33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Refactor5: edit template KAF005
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UkSource\UniversalK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Refactor5\KAF005\template_update\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,7 +53,6 @@
     <definedName name="kkkk" hidden="1">#REF!</definedName>
     <definedName name="ｌ" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ｌ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">残業申請!$A$1:$L$38</definedName>
     <definedName name="sss" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="sss" hidden="1">#REF!</definedName>
     <definedName name="Ver002001006特休残管理対応" localSheetId="0" hidden="1">#REF!</definedName>
@@ -72,21 +71,13 @@
     <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
     <definedName name="関連表" hidden="1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="1">
-  <si>
-    <t>g</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -341,7 +332,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -384,6 +375,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="20" fontId="5" fillId="2" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -497,15 +491,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -563,7 +548,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3164016" y="223630"/>
+          <a:off x="3181601" y="223630"/>
           <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
@@ -914,8 +899,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3780538" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="3798123" y="223630"/>
+          <a:ext cx="616579" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1251,7 +1236,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4405106" y="223630"/>
+          <a:off x="4430018" y="223630"/>
           <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
@@ -1595,8 +1580,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5018789" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="5043701" y="223630"/>
+          <a:ext cx="616579" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1932,7 +1917,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5643357" y="223630"/>
+          <a:off x="5675595" y="223630"/>
           <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
@@ -2641,8 +2626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
@@ -2677,11 +2662,11 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2691,11 +2676,11 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="45"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2719,8 +2704,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -2733,8 +2718,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -2747,436 +2732,422 @@
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="16"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="16"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="16"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="51"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="52"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="51"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="52"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="51"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="52"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="51"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="52"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="51"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="52"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="51"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="52"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="51"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="52"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="51"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="52"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="51"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="52"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="51"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="52"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="51"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="52"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="50"/>
-      <c r="K24" s="51"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="52"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="51"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="52"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="15"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="16"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="3.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="20"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="90" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="41"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="42"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="3.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="25"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="26"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="3.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="20"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="21"/>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="41"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="42"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="3.75" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="25"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="26"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="3.75" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="28"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="29"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="41"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="42"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="3.75" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="31"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="32"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" ht="3.75" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="28"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="29"/>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" ht="74.25" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="41"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="42"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" ht="3.75" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="31"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="32"/>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1">
@@ -3278,88 +3249,88 @@
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1">
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1">
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="33"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1">
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="33"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1">
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="33"/>
+      <c r="K48" s="33"/>
     </row>
     <row r="49" spans="2:11" ht="15" customHeight="1">
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="33"/>
     </row>
     <row r="50" spans="2:11" ht="15" customHeight="1">
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="33"/>
     </row>
     <row r="51" spans="2:11" ht="15" customHeight="1">
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="33"/>
     </row>
     <row r="52" spans="2:11" ht="15" customHeight="1"/>
     <row r="53" spans="2:11" ht="15" customHeight="1"/>
@@ -3371,8 +3342,7 @@
     <row r="59" spans="2:11" ht="15" customHeight="1"/>
     <row r="60" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="77">
-    <mergeCell ref="D12:K12"/>
+  <mergeCells count="76">
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="H24:I24"/>
@@ -3453,14 +3423,11 @@
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="91" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;R&amp;"ＭＳ ゴシック,標準"
 </oddHeader>
   </headerFooter>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="28" max="11" man="1"/>
-  </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor5: fix template v2 KAF005
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UkSource\UniversalK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiennd\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -86,14 +86,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -114,7 +114,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -332,7 +332,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -447,50 +447,59 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="11" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -540,7 +549,7 @@
         <xdr:cNvPr id="2" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -548,8 +557,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3181601" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="2807928" y="223630"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -559,7 +568,7 @@
           <xdr:cNvPr id="3" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -613,7 +622,7 @@
           <xdr:cNvPr id="4" name="直線コネクタ 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -653,7 +662,7 @@
           <xdr:cNvPr id="5" name="直線コネクタ 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -693,7 +702,7 @@
           <xdr:cNvPr id="6" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -749,7 +758,7 @@
           <xdr:cNvPr id="7" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -812,7 +821,7 @@
           <xdr:cNvPr id="8" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -891,7 +900,7 @@
         <xdr:cNvPr id="9" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -899,8 +908,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3798123" y="223630"/>
-          <a:ext cx="616579" cy="522000"/>
+          <a:off x="3357775" y="223630"/>
+          <a:ext cx="552835" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -910,7 +919,7 @@
           <xdr:cNvPr id="10" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -964,7 +973,7 @@
           <xdr:cNvPr id="11" name="直線コネクタ 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1004,7 +1013,7 @@
           <xdr:cNvPr id="12" name="直線コネクタ 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1044,7 +1053,7 @@
           <xdr:cNvPr id="13" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1100,7 +1109,7 @@
           <xdr:cNvPr id="14" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1156,7 +1165,7 @@
           <xdr:cNvPr id="15" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1228,7 +1237,7 @@
         <xdr:cNvPr id="16" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1236,8 +1245,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4430018" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="3909806" y="223630"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1247,7 +1256,7 @@
           <xdr:cNvPr id="17" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1301,7 +1310,7 @@
           <xdr:cNvPr id="18" name="直線コネクタ 17">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1341,7 +1350,7 @@
           <xdr:cNvPr id="19" name="直線コネクタ 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1381,7 +1390,7 @@
           <xdr:cNvPr id="20" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1437,7 +1446,7 @@
           <xdr:cNvPr id="21" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1500,7 +1509,7 @@
           <xdr:cNvPr id="22" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1572,7 +1581,7 @@
         <xdr:cNvPr id="23" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1580,8 +1589,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5043701" y="223630"/>
-          <a:ext cx="616579" cy="522000"/>
+          <a:off x="4456814" y="223630"/>
+          <a:ext cx="552835" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1591,7 +1600,7 @@
           <xdr:cNvPr id="24" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1645,7 +1654,7 @@
           <xdr:cNvPr id="25" name="直線コネクタ 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1685,7 +1694,7 @@
           <xdr:cNvPr id="26" name="直線コネクタ 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1725,7 +1734,7 @@
           <xdr:cNvPr id="27" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1781,7 +1790,7 @@
           <xdr:cNvPr id="28" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1837,7 +1846,7 @@
           <xdr:cNvPr id="29" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1909,7 +1918,7 @@
         <xdr:cNvPr id="30" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1917,8 +1926,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5675595" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="5008845" y="223630"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1928,7 +1937,7 @@
           <xdr:cNvPr id="31" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1982,7 +1991,7 @@
           <xdr:cNvPr id="32" name="直線コネクタ 31">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2022,7 +2031,7 @@
           <xdr:cNvPr id="33" name="直線コネクタ 32">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2062,7 +2071,7 @@
           <xdr:cNvPr id="34" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2118,7 +2127,7 @@
           <xdr:cNvPr id="35" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2181,7 +2190,7 @@
           <xdr:cNvPr id="36" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2626,20 +2635,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:I19"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="0.77734375" style="2" customWidth="1"/>
-    <col min="2" max="11" width="7.21875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="0.77734375" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="1.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
+    <col min="2" max="11" width="7.25" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.75" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="1.375" style="2" customWidth="1"/>
     <col min="17" max="17" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.44140625" style="2"/>
+    <col min="18" max="16384" width="2.5" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
@@ -2663,10 +2672,10 @@
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="34"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2677,10 +2686,10 @@
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="34"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2704,8 +2713,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -2718,8 +2727,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -2788,8 +2797,8 @@
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="50"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
@@ -2802,180 +2811,180 @@
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="39"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="52"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="52"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="39"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="52"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="52"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="39"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="52"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="52"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="39"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="52"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="39"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="52"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="39"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="52"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="39"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="52"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="39"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="52"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="39"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="52"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="39"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="52"/>
       <c r="H25" s="10"/>
       <c r="I25" s="37"/>
       <c r="J25" s="15"/>
@@ -2998,16 +3007,16 @@
     </row>
     <row r="27" spans="1:12" ht="90" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="46"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="55"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="3.75" customHeight="1">
@@ -3040,16 +3049,16 @@
     </row>
     <row r="30" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="46"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="42"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="3.75" customHeight="1">
@@ -3082,16 +3091,16 @@
     </row>
     <row r="33" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="46"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="42"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="3.75" customHeight="1">
@@ -3124,16 +3133,16 @@
     </row>
     <row r="36" spans="1:12" ht="74.25" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="46"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="42"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" ht="3.75" customHeight="1">
@@ -3343,12 +3352,60 @@
     <row r="60" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:K36"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:K30"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:K33"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:K27"/>
     <mergeCell ref="B25:C25"/>
@@ -3365,60 +3422,12 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:K33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>
@@ -3428,9 +3437,6 @@
     <oddHeader xml:space="preserve">&amp;R&amp;"ＭＳ ゴシック,標準"
 </oddHeader>
   </headerFooter>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="25" max="16383" man="1"/>
-  </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor5: fix template KAF005 2021/01/07
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiennd\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UkSource\UniversalK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -86,14 +86,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -114,7 +114,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -332,7 +332,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -375,9 +375,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="20" fontId="5" fillId="2" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -447,6 +444,15 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="11" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
@@ -491,15 +497,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -557,8 +554,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2807928" y="223630"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="3181601" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -908,8 +905,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3357775" y="223630"/>
-          <a:ext cx="552835" cy="522000"/>
+          <a:off x="3798123" y="223630"/>
+          <a:ext cx="616579" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1245,8 +1242,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3909806" y="223630"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="4430018" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1589,8 +1586,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4456814" y="223630"/>
-          <a:ext cx="552835" cy="522000"/>
+          <a:off x="5043701" y="223630"/>
+          <a:ext cx="616579" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1926,8 +1923,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5008845" y="223630"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="5675595" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -2635,20 +2632,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
-    <col min="2" max="11" width="7.25" style="2" customWidth="1"/>
-    <col min="12" max="12" width="0.75" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="1.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.77734375" style="2" customWidth="1"/>
+    <col min="2" max="11" width="7.21875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.77734375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="1.33203125" style="2" customWidth="1"/>
     <col min="17" max="17" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.5" style="2"/>
+    <col min="18" max="16384" width="2.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
@@ -2671,11 +2668,11 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="48"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2685,11 +2682,11 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="46"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2713,8 +2710,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="48"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -2727,8 +2724,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -2741,422 +2738,422 @@
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="16"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="16"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="52"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="54"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="52"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="54"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="52"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="54"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="52"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="54"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="52"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="54"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="52"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="54"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="52"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="54"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="52"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="54"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="52"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="54"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="52"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="54"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="52"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="54"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="52"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="54"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="52"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="54"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="16"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="3.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="90" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="55"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="44"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="3.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="26"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="25"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="3.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="21"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="20"/>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="42"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="44"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="3.75" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="26"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="25"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="3.75" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="29"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="28"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="42"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="3.75" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="32"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="31"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" ht="3.75" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="29"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="28"/>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" ht="74.25" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="42"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="44"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" ht="3.75" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="32"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="31"/>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1">
@@ -3258,88 +3255,88 @@
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1">
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="33"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1">
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="33"/>
-      <c r="J46" s="33"/>
-      <c r="K46" s="33"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1">
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="33"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="32"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1">
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
     </row>
     <row r="49" spans="2:11" ht="15" customHeight="1">
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="33"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="33"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
     </row>
     <row r="50" spans="2:11" ht="15" customHeight="1">
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="33"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32"/>
     </row>
     <row r="51" spans="2:11" ht="15" customHeight="1">
-      <c r="B51" s="33"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="33"/>
-      <c r="J51" s="33"/>
-      <c r="K51" s="33"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32"/>
     </row>
     <row r="52" spans="2:11" ht="15" customHeight="1"/>
     <row r="53" spans="2:11" ht="15" customHeight="1"/>
@@ -3351,7 +3348,7 @@
     <row r="59" spans="2:11" ht="15" customHeight="1"/>
     <row r="60" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="76">
+  <mergeCells count="77">
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="H24:I24"/>
@@ -3400,34 +3397,35 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B24:C24"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D12:K12"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D36:K36"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="D30:K30"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="D33:K33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Revert "Merge remote-tracking branch 'origin/TeamD/Refactor5/KAF006_New' into TeamD/Refactor5/KAF011_v1"
This reverts commit 4aa8a0ea0f6d04f4132704737a2c45c576473255, reversing
changes made to f83c589451c6101d615d3fd57fd3897e1c417bf1.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiennd\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UkSource\UniversalK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,6 +53,7 @@
     <definedName name="kkkk" hidden="1">#REF!</definedName>
     <definedName name="ｌ" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ｌ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">残業申請!$A$1:$L$38</definedName>
     <definedName name="sss" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="sss" hidden="1">#REF!</definedName>
     <definedName name="Ver002001006特休残管理対応" localSheetId="0" hidden="1">#REF!</definedName>
@@ -71,7 +72,7 @@
     <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
     <definedName name="関連表" hidden="1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,20 +81,28 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="1">
+  <si>
+    <t>g</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -114,7 +123,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -332,7 +341,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -375,9 +384,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="20" fontId="5" fillId="2" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -492,14 +498,14 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -557,8 +563,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2807928" y="223630"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="3164016" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -908,8 +914,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3357775" y="223630"/>
-          <a:ext cx="552835" cy="522000"/>
+          <a:off x="3780538" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1245,8 +1251,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3909806" y="223630"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="4405106" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1589,8 +1595,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4456814" y="223630"/>
-          <a:ext cx="552835" cy="522000"/>
+          <a:off x="5018789" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1926,8 +1932,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5008845" y="223630"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="5643357" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -2635,20 +2641,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
-    <col min="2" max="11" width="7.25" style="2" customWidth="1"/>
-    <col min="12" max="12" width="0.75" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="1.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.77734375" style="2" customWidth="1"/>
+    <col min="2" max="11" width="7.21875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.77734375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="1.33203125" style="2" customWidth="1"/>
     <col min="17" max="17" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.5" style="2"/>
+    <col min="18" max="16384" width="2.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
@@ -2671,11 +2677,11 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2685,11 +2691,11 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="46"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2713,8 +2719,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="48"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -2727,8 +2733,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -2741,422 +2747,436 @@
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="16"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="16"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="54" t="s">
+        <v>0</v>
+      </c>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="52"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="51"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="52"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="51"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="52"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="51"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="52"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="51"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="52"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="51"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="52"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="51"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="52"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="51"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="52"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="51"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="52"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="51"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="52"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="51"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="52"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="51"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="52"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="51"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="52"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="51"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="16"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="3.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="90" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="55"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="41"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="3.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="26"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="25"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="3.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="21"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="20"/>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="42"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="41"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="3.75" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="26"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="25"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="3.75" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="29"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="28"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="42"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="41"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="3.75" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="32"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="31"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" ht="3.75" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="29"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="28"/>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" ht="74.25" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="42"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="41"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" ht="3.75" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="32"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="31"/>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1">
@@ -3258,88 +3278,88 @@
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1">
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="33"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1">
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="33"/>
-      <c r="J46" s="33"/>
-      <c r="K46" s="33"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1">
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="33"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="32"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1">
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
     </row>
     <row r="49" spans="2:11" ht="15" customHeight="1">
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="33"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="33"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
     </row>
     <row r="50" spans="2:11" ht="15" customHeight="1">
-      <c r="B50" s="33"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="33"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32"/>
     </row>
     <row r="51" spans="2:11" ht="15" customHeight="1">
-      <c r="B51" s="33"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="33"/>
-      <c r="J51" s="33"/>
-      <c r="K51" s="33"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32"/>
     </row>
     <row r="52" spans="2:11" ht="15" customHeight="1"/>
     <row r="53" spans="2:11" ht="15" customHeight="1"/>
@@ -3351,7 +3371,8 @@
     <row r="59" spans="2:11" ht="15" customHeight="1"/>
     <row r="60" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="76">
+  <mergeCells count="77">
+    <mergeCell ref="D12:K12"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="H24:I24"/>
@@ -3432,11 +3453,14 @@
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="91" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;R&amp;"ＭＳ ゴシック,標準"
 </oddHeader>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="28" max="11" man="1"/>
+  </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "Merge remote-tracking branch 'origin/TeamD/Refactor5/KAF006_New' into TeamD/Refactor5/KAF011_v1""
This reverts commit a3acf9b556781bc52d31332b91a060c04f5978b5.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UkSource\UniversalK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hiennd\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,7 +53,6 @@
     <definedName name="kkkk" hidden="1">#REF!</definedName>
     <definedName name="ｌ" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ｌ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">残業申請!$A$1:$L$38</definedName>
     <definedName name="sss" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="sss" hidden="1">#REF!</definedName>
     <definedName name="Ver002001006特休残管理対応" localSheetId="0" hidden="1">#REF!</definedName>
@@ -72,7 +71,7 @@
     <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
     <definedName name="関連表" hidden="1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -81,28 +80,20 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="1">
-  <si>
-    <t>g</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -123,7 +114,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -341,7 +332,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -384,6 +375,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="20" fontId="5" fillId="2" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -498,14 +492,14 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -563,8 +557,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3164016" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="2807928" y="223630"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -914,8 +908,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3780538" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="3357775" y="223630"/>
+          <a:ext cx="552835" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1251,8 +1245,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4405106" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="3909806" y="223630"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1595,8 +1589,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5018789" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="4456814" y="223630"/>
+          <a:ext cx="552835" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1932,8 +1926,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5643357" y="223630"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="5008845" y="223630"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -2641,20 +2635,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="0.77734375" style="2" customWidth="1"/>
-    <col min="2" max="11" width="7.21875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="0.77734375" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="1.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
+    <col min="2" max="11" width="7.25" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.75" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="1.375" style="2" customWidth="1"/>
     <col min="17" max="17" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.44140625" style="2"/>
+    <col min="18" max="16384" width="2.5" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
@@ -2677,11 +2671,11 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2691,11 +2685,11 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="45"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2719,8 +2713,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -2733,8 +2727,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -2747,436 +2741,422 @@
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="16"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="16"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" s="54" t="s">
-        <v>0</v>
-      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="16"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="51"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="52"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="51"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="52"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="51"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="52"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="51"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="52"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="51"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="52"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="51"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="52"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="51"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="52"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="51"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="52"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="51"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="52"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="51"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="52"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="51"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="52"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="50"/>
-      <c r="K24" s="51"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="52"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="51"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="52"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="15"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="16"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="3.75" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="20"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="90" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="41"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="55"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="3.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="25"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="26"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="3.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="20"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="21"/>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="41"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="42"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="3.75" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="25"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="26"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="3.75" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="28"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="29"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="41"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="42"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="3.75" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="31"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="32"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" ht="3.75" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="28"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="29"/>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" ht="74.25" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="41"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="42"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" ht="3.75" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="31"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="32"/>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1">
@@ -3278,88 +3258,88 @@
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1">
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
     </row>
     <row r="46" spans="1:12" ht="15" customHeight="1">
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="33"/>
     </row>
     <row r="47" spans="1:12" ht="15" customHeight="1">
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="33"/>
     </row>
     <row r="48" spans="1:12" ht="15" customHeight="1">
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="33"/>
+      <c r="K48" s="33"/>
     </row>
     <row r="49" spans="2:11" ht="15" customHeight="1">
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="33"/>
     </row>
     <row r="50" spans="2:11" ht="15" customHeight="1">
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="33"/>
     </row>
     <row r="51" spans="2:11" ht="15" customHeight="1">
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="33"/>
     </row>
     <row r="52" spans="2:11" ht="15" customHeight="1"/>
     <row r="53" spans="2:11" ht="15" customHeight="1"/>
@@ -3371,8 +3351,7 @@
     <row r="59" spans="2:11" ht="15" customHeight="1"/>
     <row r="60" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="77">
-    <mergeCell ref="D12:K12"/>
+  <mergeCells count="76">
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="H24:I24"/>
@@ -3453,14 +3432,11 @@
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="91" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;R&amp;"ＭＳ ゴシック,標準"
 </oddHeader>
   </headerFooter>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="28" max="11" man="1"/>
-  </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor5: Fix bug #114507 KAF005
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UkSource\UniversalK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF005_残業申請\ver4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23145" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27405" windowHeight="12825"/>
   </bookViews>
   <sheets>
     <sheet name="残業申請" sheetId="29" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -435,14 +435,38 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="20" fontId="5" fillId="2" borderId="11" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="20" fontId="5" fillId="2" borderId="11" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
@@ -468,39 +492,15 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 10" xfId="2"/>
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="4"/>
@@ -546,7 +546,7 @@
         <xdr:cNvPr id="2" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -554,7 +554,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3181601" y="223630"/>
+          <a:off x="3164016" y="223630"/>
           <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
@@ -565,7 +565,7 @@
           <xdr:cNvPr id="3" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -619,7 +619,7 @@
           <xdr:cNvPr id="4" name="直線コネクタ 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -659,7 +659,7 @@
           <xdr:cNvPr id="5" name="直線コネクタ 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -699,7 +699,7 @@
           <xdr:cNvPr id="6" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -755,7 +755,7 @@
           <xdr:cNvPr id="7" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -818,7 +818,7 @@
           <xdr:cNvPr id="8" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -897,7 +897,7 @@
         <xdr:cNvPr id="9" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -905,8 +905,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3798123" y="223630"/>
-          <a:ext cx="616579" cy="522000"/>
+          <a:off x="3780538" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -916,7 +916,7 @@
           <xdr:cNvPr id="10" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -970,7 +970,7 @@
           <xdr:cNvPr id="11" name="直線コネクタ 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1010,7 +1010,7 @@
           <xdr:cNvPr id="12" name="直線コネクタ 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1050,7 +1050,7 @@
           <xdr:cNvPr id="13" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1106,7 +1106,7 @@
           <xdr:cNvPr id="14" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1162,7 +1162,7 @@
           <xdr:cNvPr id="15" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1234,7 +1234,7 @@
         <xdr:cNvPr id="16" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1242,7 +1242,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4430018" y="223630"/>
+          <a:off x="4405106" y="223630"/>
           <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
@@ -1253,7 +1253,7 @@
           <xdr:cNvPr id="17" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1307,7 +1307,7 @@
           <xdr:cNvPr id="18" name="直線コネクタ 17">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1347,7 +1347,7 @@
           <xdr:cNvPr id="19" name="直線コネクタ 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1387,7 +1387,7 @@
           <xdr:cNvPr id="20" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1443,7 +1443,7 @@
           <xdr:cNvPr id="21" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1506,7 +1506,7 @@
           <xdr:cNvPr id="22" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1578,7 +1578,7 @@
         <xdr:cNvPr id="23" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1586,8 +1586,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5043701" y="223630"/>
-          <a:ext cx="616579" cy="522000"/>
+          <a:off x="5018789" y="223630"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1597,7 +1597,7 @@
           <xdr:cNvPr id="24" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1651,7 +1651,7 @@
           <xdr:cNvPr id="25" name="直線コネクタ 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1691,7 +1691,7 @@
           <xdr:cNvPr id="26" name="直線コネクタ 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1731,7 +1731,7 @@
           <xdr:cNvPr id="27" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1787,7 +1787,7 @@
           <xdr:cNvPr id="28" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1843,7 +1843,7 @@
           <xdr:cNvPr id="29" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1915,7 +1915,7 @@
         <xdr:cNvPr id="30" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1923,7 +1923,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5675595" y="223630"/>
+          <a:off x="5643357" y="223630"/>
           <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
@@ -1934,7 +1934,7 @@
           <xdr:cNvPr id="31" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1988,7 +1988,7 @@
           <xdr:cNvPr id="32" name="直線コネクタ 31">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2028,7 +2028,7 @@
           <xdr:cNvPr id="33" name="直線コネクタ 32">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2068,7 +2068,7 @@
           <xdr:cNvPr id="34" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2124,7 +2124,7 @@
           <xdr:cNvPr id="35" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2187,7 +2187,7 @@
           <xdr:cNvPr id="36" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2632,8 +2632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:K27"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
@@ -2669,10 +2669,10 @@
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="33"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2683,10 +2683,10 @@
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="33"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2710,8 +2710,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -2724,8 +2724,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -2738,8 +2738,8 @@
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="54"/>
       <c r="D8" s="13"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -2752,8 +2752,8 @@
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="13"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -2766,8 +2766,8 @@
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="13"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -2780,8 +2780,8 @@
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="13"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -2794,196 +2794,196 @@
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="39"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="47"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="54"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="36"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="54"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="36"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="54"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="36"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="36"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="54"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="36"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="54"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="36"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="36"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="54"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="36"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="54"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="36"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="54"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="36"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="54"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="36"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="54"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="36"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="54"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="36"/>
+      <c r="I25" s="34"/>
       <c r="J25" s="14"/>
       <c r="K25" s="15"/>
       <c r="L25" s="1"/>
@@ -3004,16 +3004,16 @@
     </row>
     <row r="27" spans="1:12" ht="90" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="44"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="52"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="3.75" customHeight="1">
@@ -3046,16 +3046,16 @@
     </row>
     <row r="30" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="44"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="52"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="3.75" customHeight="1">
@@ -3088,16 +3088,16 @@
     </row>
     <row r="33" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="44"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="52"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="3.75" customHeight="1">
@@ -3130,16 +3130,16 @@
     </row>
     <row r="36" spans="1:12" ht="74.25" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="44"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="52"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" ht="3.75" customHeight="1">
@@ -3348,7 +3348,72 @@
     <row r="59" spans="2:11" ht="15" customHeight="1"/>
     <row r="60" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="77">
+  <mergeCells count="81">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:K33"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="H24:I24"/>
@@ -3365,67 +3430,6 @@
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:K12"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:K36"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:K30"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:K33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Refactor5: Fix bug #114505 KAF005
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF005_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF005_残業申請\ver4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Refactor5\KAF005\114507\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,6 +53,7 @@
     <definedName name="kkkk" hidden="1">#REF!</definedName>
     <definedName name="ｌ" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ｌ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">残業申請!$A$1:$L$36</definedName>
     <definedName name="sss" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="sss" hidden="1">#REF!</definedName>
     <definedName name="Ver002001006特休残管理対応" localSheetId="0" hidden="1">#REF!</definedName>
@@ -71,7 +72,7 @@
     <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
     <definedName name="関連表" hidden="1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -81,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -332,7 +333,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -438,16 +439,73 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="11" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -456,51 +514,9 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準 10" xfId="2"/>
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="4"/>
@@ -546,7 +562,7 @@
         <xdr:cNvPr id="2" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -565,7 +581,7 @@
           <xdr:cNvPr id="3" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -619,7 +635,7 @@
           <xdr:cNvPr id="4" name="直線コネクタ 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -659,7 +675,7 @@
           <xdr:cNvPr id="5" name="直線コネクタ 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -699,7 +715,7 @@
           <xdr:cNvPr id="6" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -755,7 +771,7 @@
           <xdr:cNvPr id="7" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -818,7 +834,7 @@
           <xdr:cNvPr id="8" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -897,7 +913,7 @@
         <xdr:cNvPr id="9" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -916,7 +932,7 @@
           <xdr:cNvPr id="10" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -970,7 +986,7 @@
           <xdr:cNvPr id="11" name="直線コネクタ 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1010,7 +1026,7 @@
           <xdr:cNvPr id="12" name="直線コネクタ 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1050,7 +1066,7 @@
           <xdr:cNvPr id="13" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1106,7 +1122,7 @@
           <xdr:cNvPr id="14" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1162,7 +1178,7 @@
           <xdr:cNvPr id="15" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1234,7 +1250,7 @@
         <xdr:cNvPr id="16" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1253,7 +1269,7 @@
           <xdr:cNvPr id="17" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1307,7 +1323,7 @@
           <xdr:cNvPr id="18" name="直線コネクタ 17">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1347,7 +1363,7 @@
           <xdr:cNvPr id="19" name="直線コネクタ 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1387,7 +1403,7 @@
           <xdr:cNvPr id="20" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1443,7 +1459,7 @@
           <xdr:cNvPr id="21" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1506,7 +1522,7 @@
           <xdr:cNvPr id="22" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1578,7 +1594,7 @@
         <xdr:cNvPr id="23" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1597,7 +1613,7 @@
           <xdr:cNvPr id="24" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1651,7 +1667,7 @@
           <xdr:cNvPr id="25" name="直線コネクタ 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1691,7 +1707,7 @@
           <xdr:cNvPr id="26" name="直線コネクタ 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1731,7 +1747,7 @@
           <xdr:cNvPr id="27" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1787,7 +1803,7 @@
           <xdr:cNvPr id="28" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1843,7 +1859,7 @@
           <xdr:cNvPr id="29" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1915,7 +1931,7 @@
         <xdr:cNvPr id="30" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1934,7 +1950,7 @@
           <xdr:cNvPr id="31" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1988,7 +2004,7 @@
           <xdr:cNvPr id="32" name="直線コネクタ 31">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2028,7 +2044,7 @@
           <xdr:cNvPr id="33" name="直線コネクタ 32">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2068,7 +2084,7 @@
           <xdr:cNvPr id="34" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2124,7 +2140,7 @@
           <xdr:cNvPr id="35" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2187,7 +2203,7 @@
           <xdr:cNvPr id="36" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2630,10 +2646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
@@ -2669,10 +2685,10 @@
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="33"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2683,10 +2699,10 @@
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="33"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="44"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2710,8 +2726,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="42"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -2724,8 +2740,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -2738,8 +2754,8 @@
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="54"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="57"/>
       <c r="D8" s="13"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -2752,8 +2768,8 @@
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="54"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="57"/>
       <c r="D9" s="13"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -2766,8 +2782,8 @@
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="13"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -2780,8 +2796,8 @@
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="54"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="13"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -2794,194 +2810,194 @@
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="47"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="55"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="36"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="45"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="36"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="45"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="36"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="45"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="36"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="45"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="36"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="45"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="36"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="45"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="36"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="45"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="36"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="45"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="36"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="45"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="36"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="45"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="36"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="45"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="36"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="45"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="45"/>
       <c r="H25" s="10"/>
       <c r="I25" s="34"/>
       <c r="J25" s="14"/>
@@ -3004,16 +3020,16 @@
     </row>
     <row r="27" spans="1:12" ht="90" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="52"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="39"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="3.75" customHeight="1">
@@ -3046,16 +3062,16 @@
     </row>
     <row r="30" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="52"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="39"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="3.75" customHeight="1">
@@ -3088,16 +3104,16 @@
     </row>
     <row r="33" spans="1:12" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="52"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="39"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="3.75" customHeight="1">
@@ -3130,30 +3146,30 @@
     </row>
     <row r="36" spans="1:12" ht="74.25" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="52"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="50"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" ht="3.75" customHeight="1">
+    <row r="37" spans="1:12" ht="15" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="31"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1">
@@ -3241,18 +3257,16 @@
       <c r="L43" s="1"/>
     </row>
     <row r="44" spans="1:12" ht="15" customHeight="1">
-      <c r="A44" s="1"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="1"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
     </row>
     <row r="45" spans="1:12" ht="15" customHeight="1">
       <c r="B45" s="32"/>
@@ -3326,18 +3340,7 @@
       <c r="J50" s="32"/>
       <c r="K50" s="32"/>
     </row>
-    <row r="51" spans="2:11" ht="15" customHeight="1">
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-    </row>
+    <row r="51" spans="2:11" ht="15" customHeight="1"/>
     <row r="52" spans="2:11" ht="15" customHeight="1"/>
     <row r="53" spans="2:11" ht="15" customHeight="1"/>
     <row r="54" spans="2:11" ht="15" customHeight="1"/>
@@ -3346,47 +3349,35 @@
     <row r="57" spans="2:11" ht="15" customHeight="1"/>
     <row r="58" spans="2:11" ht="15" customHeight="1"/>
     <row r="59" spans="2:11" ht="15" customHeight="1"/>
-    <row r="60" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:K36"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:K30"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:K33"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:K12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="F13:G13"/>
@@ -3403,33 +3394,44 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:K33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>